<commit_message>
#154: read and write vertical header tables.
</commit_message>
<xml_diff>
--- a/ecuacion-util-poi/src/test/resources/CellOneLineHeaderExcelTableWriterTest.xlsx
+++ b/ecuacion-util-poi/src/test/resources/CellOneLineHeaderExcelTableWriterTest.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yosuke.tanaka/Desktop/development/git/ecuacion-utils/ecuacion-util-poi/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A3EB3B-296E-D147-925D-A8258A76E9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD69CE4-D03C-9A4E-B1BA-F32D00F1F244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="28300" windowHeight="16640" activeTab="2" xr2:uid="{64331AC0-51A5-0346-AE3C-70EE1E686969}"/>
+    <workbookView xWindow="200" yWindow="500" windowWidth="28300" windowHeight="16640" activeTab="3" xr2:uid="{64331AC0-51A5-0346-AE3C-70EE1E686969}"/>
   </bookViews>
   <sheets>
     <sheet name="copy-from" sheetId="1" r:id="rId1"/>
     <sheet name="copy-to-normalTableTest" sheetId="2" r:id="rId2"/>
     <sheet name="copy-to-tableWithNullCellseTest" sheetId="3" r:id="rId3"/>
+    <sheet name="copy-to-verticalHeaderTableTest" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>header1</t>
     <phoneticPr fontId="1"/>
@@ -116,6 +117,9 @@
   </si>
   <si>
     <t>- table with  null cells</t>
+  </si>
+  <si>
+    <t>- vertical header table</t>
   </si>
 </sst>
 </file>
@@ -164,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +208,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FA00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,7 +284,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -309,6 +319,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -666,7 +679,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -861,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8CE56-F66A-3D48-A49A-3E8DDC126C37}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -881,4 +894,37 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A895B44-D9A1-9542-BF52-6D2B4C93D3CB}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C3" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C4" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>